<commit_message>
Retrieve data from excel sheet and use data providers to run multiple sets
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t>testname</t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -19,10 +22,19 @@
     <t>job</t>
   </si>
   <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>testPostUser</t>
+  </si>
+  <si>
     <t>Ayush</t>
   </si>
   <si>
     <t>Leader</t>
+  </si>
+  <si>
+    <t>201</t>
   </si>
 </sst>
 </file>
@@ -63,7 +75,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -90,6 +102,39 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="10"/>
@@ -102,9 +147,7 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -114,24 +157,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -179,7 +204,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -214,6 +239,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1299,14 +1327,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1316,66 +1344,84 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
+      <c r="C2" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="6"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Create groups and before and after method functions for parallel test execution
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>testname</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>201</t>
+  </si>
+  <si>
+    <t>testDeleteUser</t>
+  </si>
+  <si>
+    <t>204</t>
   </si>
 </sst>
 </file>
@@ -1368,17 +1374,25 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="A3" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">

</xml_diff>

<commit_message>
Add authentication tests for creating custom request specification
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId4"/>
+    <sheet name="AuthData" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>testname</t>
   </si>
@@ -42,6 +43,21 @@
   <si>
     <t>204</t>
   </si>
+  <si>
+    <t>formParam</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>testAuthWithClientCredentials</t>
+  </si>
+  <si>
+    <t>client_id:rest_assured_oauth_demo_app;client_secret:05c3e7b288e0f9cd2a51afa1dc660d11;grant_type:client_credentials</t>
+  </si>
+  <si>
+    <t>1711</t>
+  </si>
 </sst>
 </file>
 
@@ -67,7 +83,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,8 +96,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -204,13 +226,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -248,6 +313,24 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -269,6 +352,9 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1444,4 +1530,50 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="3" width="16.3516" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" t="s" s="14">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" t="s" s="16">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="17">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s" s="18">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modularise auth setup and token generation
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>testname</t>
   </si>
@@ -44,13 +44,25 @@
     <t>204</t>
   </si>
   <si>
-    <t>formParam</t>
+    <t>authRequired</t>
+  </si>
+  <si>
+    <t>authType</t>
+  </si>
+  <si>
+    <t>authParams</t>
   </si>
   <si>
     <t>user_id</t>
   </si>
   <si>
     <t>testAuthWithClientCredentials</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>oauth2CC</t>
   </si>
   <si>
     <t>client_id:rest_assured_oauth_demo_app;client_secret:05c3e7b288e0f9cd2a51afa1dc660d11;grant_type:client_credentials</t>
@@ -103,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -246,6 +258,21 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
         <color indexed="12"/>
       </right>
       <top style="thin">
@@ -275,7 +302,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -331,6 +358,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1537,14 +1567,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="16.3516" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="13" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1554,19 +1584,31 @@
       <c r="B1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="C1" t="s" s="15">
+      <c r="C1" t="s" s="2">
         <v>11</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s" s="15">
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s" s="17">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s" s="18">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C2" t="s" s="17">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s" s="18">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s" s="19">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename AuthorizationTests to BarnFarmTests
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -6,13 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId4"/>
-    <sheet name="AuthData" sheetId="2" r:id="rId5"/>
+    <sheet name="BarnData" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -44,7 +44,7 @@
     <t>204</t>
   </si>
   <si>
-    <t>authRequired</t>
+    <t>setAuth</t>
   </si>
   <si>
     <t>authType</t>
@@ -53,10 +53,25 @@
     <t>authParams</t>
   </si>
   <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>testAuthWithClientCredentials</t>
+    <t>setPathParams</t>
+  </si>
+  <si>
+    <t>pathParams</t>
+  </si>
+  <si>
+    <t>setHeaders</t>
+  </si>
+  <si>
+    <t>headers</t>
+  </si>
+  <si>
+    <t>setQueryParams</t>
+  </si>
+  <si>
+    <t>queryParams</t>
+  </si>
+  <si>
+    <t>testBarnUnlockWithClientCredentials</t>
   </si>
   <si>
     <t>Y</t>
@@ -68,7 +83,10 @@
     <t>client_id:rest_assured_oauth_demo_app;client_secret:05c3e7b288e0f9cd2a51afa1dc660d11;grant_type:client_credentials</t>
   </si>
   <si>
-    <t>1711</t>
+    <t>user_id:1711</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -115,7 +133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -235,6 +253,21 @@
       <top/>
       <bottom style="thin">
         <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -249,7 +282,7 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -260,11 +293,9 @@
       <right style="thin">
         <color indexed="13"/>
       </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -273,21 +304,6 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
         <color indexed="10"/>
       </right>
       <top/>
@@ -296,13 +312,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -351,7 +398,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -361,6 +408,15 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -383,8 +439,8 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1567,14 +1623,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="10" width="16.3516" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1593,23 +1649,145 @@
       <c r="E1" t="s" s="15">
         <v>13</v>
       </c>
+      <c r="F1" t="s" s="15">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s" s="15">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s" s="15">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s" s="15">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="16">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s" s="17">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s" s="17">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s" s="18">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s" s="19">
-        <v>18</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="16">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="17">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s" s="18">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s" s="18">
+        <v>24</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" t="s" s="18">
+        <v>24</v>
+      </c>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Set base url as part of header setup | Use Run Manager sheet to set up test headers and params
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -6,13 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId4"/>
-    <sheet name="BarnData" sheetId="2" r:id="rId5"/>
+    <sheet name="RunManager" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>testname</t>
   </si>
@@ -71,6 +71,9 @@
     <t>queryParams</t>
   </si>
   <si>
+    <t>base_url</t>
+  </si>
+  <si>
     <t>testBarnUnlockWithClientCredentials</t>
   </si>
   <si>
@@ -87,6 +90,17 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="13"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>http://coop.apps.symfonycasts.com</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -96,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -111,6 +125,17 @@
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="13"/>
+      <color indexed="14"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -133,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -343,13 +368,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -407,8 +445,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -417,6 +455,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -441,6 +482,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1623,14 +1665,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="10" width="16.3516" style="13" customWidth="1"/>
-    <col min="11" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="11" width="16.3516" style="13" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1664,34 +1706,40 @@
       <c r="J1" t="s" s="15">
         <v>18</v>
       </c>
+      <c r="K1" t="s" s="15">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="16">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s" s="16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s" s="16">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="17">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s" s="18">
         <v>21</v>
       </c>
-      <c r="D2" t="s" s="17">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s" s="18">
-        <v>20</v>
-      </c>
       <c r="F2" t="s" s="18">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s" s="18">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" t="s" s="18">
-        <v>24</v>
-      </c>
-      <c r="J2" s="19"/>
+        <v>25</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" t="s" s="19">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="20"/>
@@ -1704,6 +1752,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="22"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="8"/>
@@ -1716,6 +1765,7 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="7"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="8"/>
@@ -1728,6 +1778,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="7"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="8"/>
@@ -1740,6 +1791,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="7"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="8"/>
@@ -1752,6 +1804,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="7"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="8"/>
@@ -1764,6 +1817,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="7"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="8"/>
@@ -1776,6 +1830,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="7"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="10"/>
@@ -1788,8 +1843,12 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
+      <c r="K10" s="23"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" location="" tooltip="" display="http://coop.apps.symfonycasts.com"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Create before and after method implementations for tests
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -74,7 +74,7 @@
     <t>base_url</t>
   </si>
   <si>
-    <t>testBarnUnlockWithClientCredentials</t>
+    <t>Barn Farm Tests</t>
   </si>
   <si>
     <t>Y</t>
@@ -102,6 +102,20 @@
       <t>http://coop.apps.symfonycasts.com</t>
     </r>
   </si>
+  <si>
+    <t>User CRUD Tests</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://reqres.in</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -110,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -136,6 +150,12 @@
       <sz val="13"/>
       <color indexed="14"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="14"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -387,7 +407,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -444,17 +464,23 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1665,14 +1691,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="11" width="16.3516" style="13" customWidth="1"/>
-    <col min="12" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="13" width="16.3516" style="13" customWidth="1"/>
+    <col min="14" max="16384" width="16.3516" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1709,6 +1735,8 @@
       <c r="K1" t="s" s="15">
         <v>19</v>
       </c>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="16">
@@ -1740,22 +1768,30 @@
       <c r="K2" t="s" s="19">
         <v>26</v>
       </c>
+      <c r="L2" s="19"/>
+      <c r="M2" s="20"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="20"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="A3" t="s" s="21">
+        <v>27</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="3"/>
+      <c r="J3" s="23"/>
+      <c r="K3" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1765,7 +1801,9 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="4"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="8"/>
@@ -1779,6 +1817,8 @@
       <c r="I5" s="9"/>
       <c r="J5" s="7"/>
       <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="8"/>
@@ -1792,6 +1832,8 @@
       <c r="I6" s="9"/>
       <c r="J6" s="7"/>
       <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="8"/>
@@ -1805,6 +1847,8 @@
       <c r="I7" s="9"/>
       <c r="J7" s="7"/>
       <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="8"/>
@@ -1818,6 +1862,8 @@
       <c r="I8" s="9"/>
       <c r="J8" s="7"/>
       <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="8"/>
@@ -1831,6 +1877,8 @@
       <c r="I9" s="9"/>
       <c r="J9" s="7"/>
       <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="10"/>
@@ -1843,11 +1891,14 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
-      <c r="K10" s="23"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" location="" tooltip="" display="http://coop.apps.symfonycasts.com"/>
+    <hyperlink ref="K3" r:id="rId2" location="" tooltip="" display="https://reqres.in"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Use createUser flag to handle user creation/deletion
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>testname</t>
   </si>
@@ -26,6 +26,9 @@
     <t>expected</t>
   </si>
   <si>
+    <t>createUser</t>
+  </si>
+  <si>
     <t>testPostUser</t>
   </si>
   <si>
@@ -38,12 +41,18 @@
     <t>201</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>testDeleteUser</t>
   </si>
   <si>
     <t>204</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>setAuth</t>
   </si>
   <si>
@@ -77,9 +86,6 @@
     <t>Barn Farm Tests</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>oauth2CC</t>
   </si>
   <si>
@@ -87,9 +93,6 @@
   </si>
   <si>
     <t>user_id:1711</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <r>
@@ -407,7 +410,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -417,10 +420,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -451,9 +454,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -480,7 +480,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1596,37 +1602,43 @@
       <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" t="s" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="E2" t="s" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="E3" t="s" s="4">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="5"/>
@@ -1706,89 +1718,89 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s" s="15">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s" s="15">
         <v>15</v>
       </c>
-      <c r="H1" t="s" s="15">
+      <c r="E1" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="I1" t="s" s="15">
+      <c r="F1" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="J1" t="s" s="15">
+      <c r="G1" t="s" s="3">
         <v>18</v>
       </c>
-      <c r="K1" t="s" s="15">
+      <c r="H1" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="I1" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s" s="3">
+        <v>22</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="16">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s" s="16">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s" s="16">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s" s="17">
+      <c r="A2" t="s" s="15">
         <v>23</v>
       </c>
-      <c r="E2" t="s" s="18">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s" s="18">
+      <c r="B2" t="s" s="15">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s" s="15">
         <v>24</v>
       </c>
-      <c r="G2" t="s" s="18">
+      <c r="D2" t="s" s="16">
         <v>25</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" t="s" s="18">
-        <v>25</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" t="s" s="19">
+      <c r="E2" t="s" s="17">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="17">
         <v>26</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="20"/>
+      <c r="G2" t="s" s="17">
+        <v>9</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" t="s" s="17">
+        <v>9</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" t="s" s="18">
+        <v>27</v>
+      </c>
+      <c r="L2" s="18"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="21">
-        <v>27</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="A3" t="s" s="20">
+        <v>28</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
       <c r="K3" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="24"/>
@@ -1801,9 +1813,9 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="8"/>
@@ -1816,9 +1828,9 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="8"/>
@@ -1831,9 +1843,9 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="8"/>
@@ -1846,9 +1858,9 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="8"/>
@@ -1861,9 +1873,9 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="7"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="8"/>
@@ -1876,9 +1888,9 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="10"/>
@@ -1891,9 +1903,9 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Read expected value from excelsheet for BarnTests
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -6,13 +6,14 @@
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId4"/>
-    <sheet name="RunManager" sheetId="2" r:id="rId5"/>
+    <sheet name="BarnData" sheetId="2" r:id="rId5"/>
+    <sheet name="RunManager" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>testname</t>
   </si>
@@ -51,6 +52,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>testBarnUnlockWithClientCredentials</t>
+  </si>
+  <si>
+    <t>200</t>
   </si>
   <si>
     <t>setAuth</t>
@@ -181,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -305,18 +312,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
+      <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -330,8 +333,52 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -341,18 +388,20 @@
       <right style="thin">
         <color indexed="13"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -362,38 +411,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -404,13 +422,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -426,60 +457,78 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -489,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -512,8 +561,8 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
@@ -1644,50 +1693,50 @@
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="7"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1703,209 +1752,311 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="14" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" t="s" s="15">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" ht="17.3" customHeight="1">
+      <c r="A2" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s" s="19">
+        <v>14</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="16.3516" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="16.3516" style="13" customWidth="1"/>
+    <col min="1" max="13" width="16.3516" style="23" customWidth="1"/>
+    <col min="14" max="16384" width="16.3516" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="14">
+      <c r="A1" t="s" s="15">
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s" s="3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I1" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J1" t="s" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="15">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s" s="15">
+      <c r="A2" t="s" s="24">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s" s="24">
         <v>12</v>
       </c>
-      <c r="C2" t="s" s="15">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s" s="16">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s" s="17">
+      <c r="C2" t="s" s="24">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s" s="19">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s" s="25">
         <v>12</v>
       </c>
-      <c r="F2" t="s" s="17">
-        <v>26</v>
-      </c>
-      <c r="G2" t="s" s="17">
+      <c r="F2" t="s" s="25">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s" s="25">
         <v>9</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" t="s" s="17">
+      <c r="H2" s="25"/>
+      <c r="I2" t="s" s="25">
         <v>9</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" t="s" s="18">
-        <v>27</v>
-      </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="19"/>
+      <c r="J2" s="25"/>
+      <c r="K2" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="20">
-        <v>28</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="A3" t="s" s="28">
+        <v>30</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="22"/>
+      <c r="J3" s="17"/>
       <c r="K3" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+        <v>31</v>
+      </c>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="24"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="7"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Optimise DataProviderUtils to reduce number of methods based on tests
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -90,7 +90,7 @@
     <t>base_url</t>
   </si>
   <si>
-    <t>Barn Farm Tests</t>
+    <t>BarnFarmTests</t>
   </si>
   <si>
     <t>oauth2CC</t>
@@ -113,7 +113,7 @@
     </r>
   </si>
   <si>
-    <t>User CRUD Tests</t>
+    <t>UserCRUDTests</t>
   </si>
   <si>
     <r>

</xml_diff>

<commit_message>
Add test for adding a book assigned to a user
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -8,12 +8,14 @@
     <sheet name="UserData" sheetId="1" r:id="rId4"/>
     <sheet name="BarnData" sheetId="2" r:id="rId5"/>
     <sheet name="RunManager" sheetId="3" r:id="rId6"/>
+    <sheet name="BookData_Main" sheetId="4" r:id="rId7"/>
+    <sheet name="BookData_Isbn" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>testname</t>
   </si>
@@ -60,28 +62,16 @@
     <t>200</t>
   </si>
   <si>
-    <t>setAuth</t>
-  </si>
-  <si>
     <t>authType</t>
   </si>
   <si>
     <t>authParams</t>
   </si>
   <si>
-    <t>setPathParams</t>
-  </si>
-  <si>
     <t>pathParams</t>
   </si>
   <si>
-    <t>setHeaders</t>
-  </si>
-  <si>
     <t>headers</t>
-  </si>
-  <si>
-    <t>setQueryParams</t>
   </si>
   <si>
     <t>queryParams</t>
@@ -125,6 +115,47 @@
       </rPr>
       <t>https://reqres.in</t>
     </r>
+  </si>
+  <si>
+    <t>BookTests</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="14"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://demoqa.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>testAddListOfBooks</t>
+  </si>
+  <si>
+    <t>e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
+  </si>
+  <si>
+    <t>isbn</t>
+  </si>
+  <si>
+    <t>9781449325862</t>
+  </si>
+  <si>
+    <t>9781449331818</t>
+  </si>
+  <si>
+    <t>9781449337711</t>
+  </si>
+  <si>
+    <t>9781449365035</t>
   </si>
 </sst>
 </file>
@@ -188,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -435,13 +466,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -535,10 +603,37 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1854,14 +1949,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="16.3516" style="23" customWidth="1"/>
-    <col min="14" max="16384" width="16.3516" style="23" customWidth="1"/>
+    <col min="1" max="9" width="16.3516" style="23" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -1874,7 +1969,7 @@
       <c r="C1" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" t="s" s="3">
         <v>17</v>
       </c>
       <c r="E1" t="s" s="3">
@@ -1886,87 +1981,61 @@
       <c r="G1" t="s" s="3">
         <v>20</v>
       </c>
-      <c r="H1" t="s" s="3">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s" s="3">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s" s="3">
-        <v>24</v>
-      </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="24">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s" s="25">
+        <v>24</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" t="s" s="26">
         <v>25</v>
       </c>
-      <c r="B2" t="s" s="24">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s" s="24">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s" s="19">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s" s="25">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s" s="25">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s" s="25">
-        <v>9</v>
-      </c>
-      <c r="H2" s="25"/>
-      <c r="I2" t="s" s="25">
-        <v>9</v>
-      </c>
-      <c r="J2" s="25"/>
-      <c r="K2" t="s" s="26">
-        <v>29</v>
-      </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="28">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="17"/>
-      <c r="K3" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
+      <c r="F3" s="17"/>
+      <c r="G3" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="A4" t="s" s="30">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s" s="31">
+        <v>29</v>
+      </c>
+      <c r="C4" s="31"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
+      <c r="F4" s="8"/>
+      <c r="G4" t="s" s="3">
+        <v>30</v>
+      </c>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="9"/>
@@ -1974,14 +2043,10 @@
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="9"/>
@@ -1989,14 +2054,10 @@
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="9"/>
@@ -2004,14 +2065,10 @@
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="9"/>
@@ -2019,14 +2076,10 @@
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="9"/>
@@ -2034,14 +2087,10 @@
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
@@ -2049,19 +2098,16 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" location="" tooltip="" display="http://coop.apps.symfonycasts.com"/>
-    <hyperlink ref="K3" r:id="rId2" location="" tooltip="" display="https://reqres.in"/>
+    <hyperlink ref="G2" r:id="rId1" location="" tooltip="" display="http://coop.apps.symfonycasts.com"/>
+    <hyperlink ref="G3" r:id="rId2" location="" tooltip="" display="https://reqres.in"/>
+    <hyperlink ref="G4" r:id="rId3" location="" tooltip="" display="https://demoqa.com/"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2069,4 +2115,189 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13" customHeight="1">
+      <c r="A1" t="s" s="35">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="35">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s" s="36">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" ht="13" customHeight="1">
+      <c r="A2" t="s" s="35">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s" s="35">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s" s="37">
+        <v>8</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.65" customHeight="1">
+      <c r="A1" t="s" s="39">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="35">
+        <v>34</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" ht="13.65" customHeight="1">
+      <c r="A2" t="s" s="39">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s" s="35">
+        <v>35</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" ht="13.65" customHeight="1">
+      <c r="A3" t="s" s="39">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s" s="35">
+        <v>36</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" t="s" s="39">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s" s="35">
+        <v>37</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" ht="13.65" customHeight="1">
+      <c r="A5" t="s" s="39">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="35">
+        <v>38</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Use Base64 encryption to mask sensitive data
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -86,7 +86,7 @@
     <t>oauth2CC</t>
   </si>
   <si>
-    <t>client_id:rest_assured_oauth_demo_app;client_secret:05c3e7b288e0f9cd2a51afa1dc660d11;grant_type:client_credentials</t>
+    <t>client_id:cmVzdF9hc3N1cmVkX29hdXRoX2RlbW9fYXBw;client_secret:MDVjM2U3YjI4OGUwZjljZDJhNTFhZmExZGM2NjBkMTE=;grant_type:Y2xpZW50X2NyZWRlbnRpYWxz</t>
   </si>
   <si>
     <t>user_id:1711</t>
@@ -120,7 +120,7 @@
     <t>BookTests</t>
   </si>
   <si>
-    <t>basic</t>
+    <t>QmFzaWMgYldWeVgyZHlaWGs2VTJobGNHaGxjbVJBTVRJeg==</t>
   </si>
   <si>
     <r>
@@ -2024,12 +2024,12 @@
       <c r="A4" t="s" s="30">
         <v>28</v>
       </c>
-      <c r="B4" t="s" s="31">
-        <v>29</v>
-      </c>
+      <c r="B4" s="31"/>
       <c r="C4" s="31"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="E4" t="s" s="31">
+        <v>29</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" t="s" s="3">
         <v>30</v>

</xml_diff>

<commit_message>
Add afterMethod setup for BookTests
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>testname</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
+  </si>
+  <si>
+    <t>userId:e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
   </si>
   <si>
     <t>isbn</t>
@@ -219,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -485,10 +488,34 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -509,7 +536,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -621,6 +648,12 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -630,10 +663,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2122,14 +2155,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="34" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="34" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="34" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13" customHeight="1">
@@ -2140,10 +2173,13 @@
         <v>31</v>
       </c>
       <c r="C1" t="s" s="36">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s" s="37">
         <v>3</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="17"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" ht="13" customHeight="1">
       <c r="A2" t="s" s="35">
@@ -2152,67 +2188,78 @@
       <c r="B2" t="s" s="35">
         <v>33</v>
       </c>
-      <c r="C2" t="s" s="37">
+      <c r="C2" t="s" s="38">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s" s="39">
         <v>8</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="8"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2228,70 +2275,105 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="38" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="40" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="39">
+      <c r="A1" t="s" s="41">
         <v>0</v>
       </c>
       <c r="B1" t="s" s="35">
-        <v>34</v>
-      </c>
-      <c r="C1" s="40"/>
+        <v>35</v>
+      </c>
+      <c r="C1" s="42"/>
       <c r="D1" s="6"/>
       <c r="E1" s="17"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="39">
+      <c r="A2" t="s" s="41">
         <v>32</v>
       </c>
       <c r="B2" t="s" s="35">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="10"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="39">
+      <c r="A3" t="s" s="41">
         <v>32</v>
       </c>
       <c r="B3" t="s" s="35">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="10"/>
       <c r="E3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="39">
+      <c r="A4" t="s" s="41">
         <v>32</v>
       </c>
       <c r="B4" t="s" s="35">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="10"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="39">
+      <c r="A5" t="s" s="41">
         <v>32</v>
       </c>
       <c r="B5" t="s" s="35">
-        <v>38</v>
-      </c>
-      <c r="C5" s="41"/>
+        <v>39</v>
+      </c>
+      <c r="C5" s="43"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" ht="13.65" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" ht="13.65" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" ht="13.65" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" ht="13.65" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Optimize setParam and setAuth methods in RequestSpecBuilder
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -120,6 +120,9 @@
     <t>BookTests</t>
   </si>
   <si>
+    <t>userId:e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
+  </si>
+  <si>
     <t>authorization:QmFzaWMgYldWeVgyZHlaWGs2VTJobGNHaGxjbVJBTVRJeg==;accept:YXBwbGljYXRpb24vanNvbg==</t>
   </si>
   <si>
@@ -141,9 +144,6 @@
   </si>
   <si>
     <t>e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
-  </si>
-  <si>
-    <t>userId:e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
   </si>
   <si>
     <t>isbn</t>
@@ -489,11 +489,22 @@
         <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -505,17 +516,6 @@
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -536,7 +536,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -651,19 +651,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2059,13 +2053,15 @@
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
-      <c r="D4" s="10"/>
+      <c r="D4" t="s" s="31">
+        <v>29</v>
+      </c>
       <c r="E4" t="s" s="31">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" t="s" s="3">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -2155,14 +2151,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="34" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="34" customWidth="1"/>
+    <col min="1" max="3" width="16.3516" style="34" customWidth="1"/>
+    <col min="4" max="16384" width="16.3516" style="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13" customHeight="1">
@@ -2170,96 +2166,62 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="35">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s" s="36">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s" s="37">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="17"/>
     </row>
     <row r="2" ht="13" customHeight="1">
       <c r="A2" t="s" s="35">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s" s="35">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s" s="38">
         <v>34</v>
       </c>
-      <c r="D2" t="s" s="39">
+      <c r="C2" t="s" s="37">
         <v>8</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="8"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
+      <c r="C10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2281,24 +2243,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="40" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="40" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="41">
+      <c r="A1" t="s" s="39">
         <v>0</v>
       </c>
       <c r="B1" t="s" s="35">
         <v>35</v>
       </c>
-      <c r="C1" s="42"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="6"/>
       <c r="E1" s="17"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="41">
-        <v>32</v>
+      <c r="A2" t="s" s="39">
+        <v>33</v>
       </c>
       <c r="B2" t="s" s="35">
         <v>36</v>
@@ -2308,8 +2270,8 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="41">
-        <v>32</v>
+      <c r="A3" t="s" s="39">
+        <v>33</v>
       </c>
       <c r="B3" t="s" s="35">
         <v>37</v>
@@ -2319,8 +2281,8 @@
       <c r="E3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="41">
-        <v>32</v>
+      <c r="A4" t="s" s="39">
+        <v>33</v>
       </c>
       <c r="B4" t="s" s="35">
         <v>38</v>
@@ -2330,13 +2292,13 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="41">
-        <v>32</v>
+      <c r="A5" t="s" s="39">
+        <v>33</v>
       </c>
       <c r="B5" t="s" s="35">
         <v>39</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>

</xml_diff>

<commit_message>
Add setQueryParams method to set request query params
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -120,10 +120,10 @@
     <t>BookTests</t>
   </si>
   <si>
-    <t>userId:e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
-  </si>
-  <si>
     <t>authorization:QmFzaWMgYldWeVgyZHlaWGs2VTJobGNHaGxjbVJBTVRJeg==;accept:YXBwbGljYXRpb24vanNvbg==</t>
+  </si>
+  <si>
+    <t>UserId:e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
   </si>
   <si>
     <r>
@@ -536,7 +536,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -631,6 +631,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2053,18 +2056,18 @@
       </c>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
-      <c r="D4" t="s" s="31">
+      <c r="D4" s="31"/>
+      <c r="E4" t="s" s="31">
         <v>29</v>
       </c>
-      <c r="E4" t="s" s="31">
+      <c r="F4" t="s" s="32">
         <v>30</v>
       </c>
-      <c r="F4" s="8"/>
       <c r="G4" t="s" s="3">
         <v>31</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="9"/>
@@ -2073,9 +2076,9 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="9"/>
@@ -2084,9 +2087,9 @@
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="9"/>
@@ -2095,9 +2098,9 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="9"/>
@@ -2106,9 +2109,9 @@
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="9"/>
@@ -2117,9 +2120,9 @@
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
@@ -2128,9 +2131,9 @@
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2151,77 +2154,97 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="16.3516" style="34" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="34" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="35" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13" customHeight="1">
-      <c r="A1" t="s" s="35">
+      <c r="A1" t="s" s="36">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="35">
+      <c r="B1" t="s" s="36">
         <v>32</v>
       </c>
-      <c r="C1" t="s" s="36">
+      <c r="C1" t="s" s="37">
         <v>3</v>
       </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" ht="13" customHeight="1">
-      <c r="A2" t="s" s="35">
+      <c r="A2" t="s" s="36">
         <v>33</v>
       </c>
-      <c r="B2" t="s" s="35">
+      <c r="B2" t="s" s="36">
         <v>34</v>
       </c>
-      <c r="C2" t="s" s="37">
+      <c r="C2" t="s" s="38">
         <v>8</v>
       </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
       <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
       <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="13"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -2243,26 +2266,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="38" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="39" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="39">
+      <c r="A1" t="s" s="40">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="35">
+      <c r="B1" t="s" s="36">
         <v>35</v>
       </c>
-      <c r="C1" s="40"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="6"/>
       <c r="E1" s="17"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="39">
+      <c r="A2" t="s" s="40">
         <v>33</v>
       </c>
-      <c r="B2" t="s" s="35">
+      <c r="B2" t="s" s="36">
         <v>36</v>
       </c>
       <c r="C2" s="20"/>
@@ -2270,10 +2293,10 @@
       <c r="E2" s="8"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="39">
+      <c r="A3" t="s" s="40">
         <v>33</v>
       </c>
-      <c r="B3" t="s" s="35">
+      <c r="B3" t="s" s="36">
         <v>37</v>
       </c>
       <c r="C3" s="20"/>
@@ -2281,10 +2304,10 @@
       <c r="E3" s="8"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="39">
+      <c r="A4" t="s" s="40">
         <v>33</v>
       </c>
-      <c r="B4" t="s" s="35">
+      <c r="B4" t="s" s="36">
         <v>38</v>
       </c>
       <c r="C4" s="20"/>
@@ -2292,13 +2315,13 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="39">
+      <c r="A5" t="s" s="40">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="35">
+      <c r="B5" t="s" s="36">
         <v>39</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
     </row>

</xml_diff>

<commit_message>
Read basic auth from run manager for book tests
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>testname</t>
   </si>
@@ -120,7 +120,10 @@
     <t>BookTests</t>
   </si>
   <si>
-    <t>authorization:QmFzaWMgYldWeVgyZHlaWGs2VTJobGNHaGxjbVJBTVRJeg==;accept:YXBwbGljYXRpb24vanNvbg==</t>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>bWVyX2dyZXk=:U2hlcGhlcmRAMTIz</t>
   </si>
   <si>
     <t>UserId:e42776ba-dd4e-4e5c-8f30-61b73d688f55</t>
@@ -2054,17 +2057,19 @@
       <c r="A4" t="s" s="30">
         <v>28</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" t="s" s="31">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s" s="31">
+        <v>30</v>
+      </c>
       <c r="D4" s="31"/>
-      <c r="E4" t="s" s="31">
-        <v>29</v>
-      </c>
+      <c r="E4" s="31"/>
       <c r="F4" t="s" s="32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s" s="3">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="33"/>
       <c r="I4" s="33"/>
@@ -2169,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="36">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s" s="37">
         <v>3</v>
@@ -2179,10 +2184,10 @@
     </row>
     <row r="2" ht="13" customHeight="1">
       <c r="A2" t="s" s="36">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="36">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s" s="38">
         <v>8</v>
@@ -2275,7 +2280,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="36">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="41"/>
       <c r="D1" s="6"/>
@@ -2283,10 +2288,10 @@
     </row>
     <row r="2" ht="13.65" customHeight="1">
       <c r="A2" t="s" s="40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s" s="36">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="10"/>
@@ -2294,10 +2299,10 @@
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" t="s" s="40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s" s="36">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="10"/>
@@ -2305,10 +2310,10 @@
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" t="s" s="40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s" s="36">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="10"/>
@@ -2316,10 +2321,10 @@
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" t="s" s="40">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s" s="36">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="12"/>

</xml_diff>

<commit_message>
Use factory and strategy patterns to identify auth mechanism at runtime
</commit_message>
<xml_diff>
--- a/src/main/resources/Users.xlsx
+++ b/src/main/resources/Users.xlsx
@@ -83,7 +83,7 @@
     <t>BarnFarmTests</t>
   </si>
   <si>
-    <t>oauth2CC</t>
+    <t>oAuth2CC</t>
   </si>
   <si>
     <t>client_id:cmVzdF9hc3N1cmVkX29hdXRoX2RlbW9fYXBw;client_secret:MDVjM2U3YjI4OGUwZjljZDJhNTFhZmExZGM2NjBkMTE=;grant_type:Y2xpZW50X2NyZWRlbnRpYWxz</t>
@@ -120,7 +120,7 @@
     <t>BookTests</t>
   </si>
   <si>
-    <t>basic</t>
+    <t>Basic</t>
   </si>
   <si>
     <t>bWVyX2dyZXk=:U2hlcGhlcmRAMTIz</t>

</xml_diff>